<commit_message>
//small changes check version code. In windows it is necessary to have the file qopensslbackend.dll in a subdirectory 'tls' from where the exe is. openssl must be installed in msys
</commit_message>
<xml_diff>
--- a/auxfiles/GSSHApedotransfer.xlsx
+++ b/auxfiles/GSSHApedotransfer.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF78315C-80B6-4CF3-AB92-44E271D2D1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0042F27E-F9C7-4078-8744-3EE8C7F3F447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="20520" windowHeight="12540" xr2:uid="{EE7E3014-B43F-4E75-BCA9-657834F4F7BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{EE7E3014-B43F-4E75-BCA9-657834F4F7BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tuflow" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Sand</t>
   </si>
@@ -331,6 +332,48 @@
   <si>
     <t>ln(bub)</t>
   </si>
+  <si>
+    <t>https://wiki.tuflow.com/Green-Ampt_Infiltration_Parameters#Capillary_Suction_Head</t>
+  </si>
+  <si>
+    <t>Table 1 USDA Soil types for the Green-Ampt Infiltration Method (from Rawls, W, J, Brakesiek &amp; Miller, N, 1983, ‘Green-Ampt infiltration parameters from soils data’, Journal of Hydraulic Engineering, vol 109, 62-71.)</t>
+  </si>
+  <si>
+    <t>USDA Soil Type</t>
+  </si>
+  <si>
+    <t>Suction (mm)</t>
+  </si>
+  <si>
+    <t>Hydraulic Conductivity (mm/hr)</t>
+  </si>
+  <si>
+    <t>Porosity (Fraction)</t>
+  </si>
+  <si>
+    <t>Silty Clay</t>
+  </si>
+  <si>
+    <t>Sandy Clay</t>
+  </si>
+  <si>
+    <t>Clay Loam</t>
+  </si>
+  <si>
+    <t>Silty Clay Loam</t>
+  </si>
+  <si>
+    <t>Sandy Clay Loam</t>
+  </si>
+  <si>
+    <t>Silt Loam</t>
+  </si>
+  <si>
+    <t>Sandy Loam</t>
+  </si>
+  <si>
+    <t>Loamy Sand</t>
+  </si>
 </sst>
 </file>
 
@@ -478,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -506,6 +549,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -875,6 +921,519 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1958512127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5783464566929137E-2"/>
+                  <c:y val="-0.36051727909011372"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nl-NL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>tuflow!$D$8:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>tuflow!$F$8:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>316.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>292.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>218.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>166.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CFDC-4EB3-B0EE-760654AAC9A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="477547440"/>
+        <c:axId val="477531120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="477547440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>Ksat mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477531120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="477531120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nl-NL"/>
+                  <a:t>suction mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477547440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4479,6 +5038,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5315,6 +5914,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9751,16 +10866,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>2858</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>231457</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>223838</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>18097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>307658</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>88582</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9860,15 +10975,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9896,10 +11011,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>331470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED2C10EF-9BA0-7E37-C45F-D3B94FBD3147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9937,7 +11093,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -10043,7 +11199,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -10185,7 +11341,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10195,30 +11351,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC7A993-96B8-4AA6-8EF4-C236C394CA84}">
   <dimension ref="F1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="1" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F1" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="3" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="3" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="6:29" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="6:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="F4" s="12" t="s">
         <v>11</v>
       </c>
@@ -10254,7 +11410,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="6:29" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="6:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F5" s="12"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -10286,7 +11442,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="6:29" ht="30" x14ac:dyDescent="0.45">
+    <row r="6" spans="6:29" ht="45" x14ac:dyDescent="0.3">
       <c r="F6" s="12"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -10349,7 +11505,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="7" spans="6:29" x14ac:dyDescent="0.3">
       <c r="G7" s="6" t="s">
         <v>43</v>
       </c>
@@ -10363,7 +11519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="8" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
@@ -10443,7 +11599,7 @@
         <v>1.9823798288367047</v>
       </c>
     </row>
-    <row r="9" spans="6:29" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
@@ -10523,7 +11679,7 @@
         <v>2.1621729392773008</v>
       </c>
     </row>
-    <row r="10" spans="6:29" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
@@ -10603,7 +11759,7 @@
         <v>2.6851226964585053</v>
       </c>
     </row>
-    <row r="11" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="11" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
@@ -10683,7 +11839,7 @@
         <v>2.411439497906128</v>
       </c>
     </row>
-    <row r="12" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="12" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
@@ -10763,7 +11919,7 @@
         <v>3.0344721018699214</v>
       </c>
     </row>
-    <row r="13" spans="6:29" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10843,7 +11999,7 @@
         <v>3.3350575791576103</v>
       </c>
     </row>
-    <row r="14" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="14" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
@@ -10923,7 +12079,7 @@
         <v>3.2538567937634464</v>
       </c>
     </row>
-    <row r="15" spans="6:29" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
@@ -11003,7 +12159,7 @@
         <v>3.4830845411343394</v>
       </c>
     </row>
-    <row r="16" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="16" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
@@ -11083,7 +12239,7 @@
         <v>3.3731407838796299</v>
       </c>
     </row>
-    <row r="17" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="17" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
@@ -11163,7 +12319,7 @@
         <v>3.5319332036512097</v>
       </c>
     </row>
-    <row r="18" spans="6:29" x14ac:dyDescent="0.45">
+    <row r="18" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
         <v>10</v>
       </c>
@@ -11258,12 +12414,207 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A951CB-376E-470D-B863-51AF8494E0A0}">
+  <dimension ref="B3:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>316.3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>292.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.309</v>
+      </c>
+      <c r="F11" s="2">
+        <v>208.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.432</v>
+      </c>
+      <c r="F12" s="2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="F13" s="2">
+        <v>218.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>166.8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.434</v>
+      </c>
+      <c r="F15" s="2">
+        <v>88.9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="F16" s="2">
+        <v>110.1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>117.8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F18" s="2">
+        <v>49.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11496,27 +12847,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2FDDBA-8E4A-41B0-9357-134C9F5B7B79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e80448a-be4d-46ae-83bb-e2adae7741fa"/>
-    <ds:schemaRef ds:uri="c2fb78ee-7f80-47d5-98b2-7e891369b7bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11541,9 +12882,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2FDDBA-8E4A-41B0-9357-134C9F5B7B79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e80448a-be4d-46ae-83bb-e2adae7741fa"/>
+    <ds:schemaRef ds:uri="c2fb78ee-7f80-47d5-98b2-7e891369b7bb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>